<commit_message>
New installer generation for version 1.2
</commit_message>
<xml_diff>
--- a/validation/scenary_3.xlsx
+++ b/validation/scenary_3.xlsx
@@ -13,7 +13,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>experiment 3</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>ESA Kiruna Ground Station Rx</t>
+  </si>
+  <si>
+    <t>IntervalNumber</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>StartOrbit</t>
+  </si>
+  <si>
+    <t>EndOrbit</t>
+  </si>
   <si>
     <t>Source</t>
   </si>
@@ -93,48 +123,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>47844.991770833331</v>
+        <v>47844.479861111111</v>
       </c>
       <c r="E2" s="1">
-        <v>47845.030312499999</v>
+        <v>47844.512499999997</v>
       </c>
       <c r="F2" s="0">
-        <v>3330</v>
+        <v>2820</v>
       </c>
       <c r="G2" s="0">
         <v>1</v>
@@ -145,80 +175,80 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0">
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>47845.390034722222</v>
+        <v>47845.478125000001</v>
       </c>
       <c r="E3" s="1">
-        <v>47845.595243055555</v>
+        <v>47845.511111111111</v>
       </c>
       <c r="F3" s="0">
-        <v>17730</v>
+        <v>2850</v>
       </c>
       <c r="G3" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0">
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>47845.986562500002</v>
+        <v>47846.476388888892</v>
       </c>
       <c r="E4" s="1">
-        <v>47846.028229166666</v>
+        <v>47846.509722222225</v>
       </c>
       <c r="F4" s="0">
-        <v>3600</v>
+        <v>2880</v>
       </c>
       <c r="G4" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0">
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>47846.388645833336</v>
+        <v>47847.474652777775</v>
       </c>
       <c r="E5" s="1">
-        <v>47846.593854166669</v>
+        <v>47847.508333333331</v>
       </c>
       <c r="F5" s="0">
-        <v>17730</v>
+        <v>2910</v>
       </c>
       <c r="G5" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H5" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">

</xml_diff>